<commit_message>
J file for SOAPRA corrected
The JNO2 value was missing, causing ode_solv to crash, so rectified now
</commit_message>
<xml_diff>
--- a/PyCHAM/input/auto_call_test/J_values.xlsx
+++ b/PyCHAM/input/auto_call_test/J_values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/PyCHAM/PyCHAM/input/auto_call_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D39B4A-D092-F840-9F30-4EF1CBB8F162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67873AF-8E7E-FE44-96E7-46479DFB7429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9220" yWindow="5560" windowWidth="19820" windowHeight="13060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -436,7 +436,9 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>6.7790000000000003E-3</v>
+      </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>